<commit_message>
ajout des diagrammes de classes
</commit_message>
<xml_diff>
--- a/Admimistatif/Planning.xlsx
+++ b/Admimistatif/Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damien.gygi\Documents\HES d'été DLM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lancelot\Documents\HEARC3EME\HeArcETE\Depot\Runner\Admimistatif\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -212,12 +212,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -232,6 +226,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +523,7 @@
   <dimension ref="B2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,327 +532,327 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>42607</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>42608</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>42611</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>42612</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>42613</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="7">
         <v>42614</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>42615</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
         <v>42618</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="7">
         <v>42619</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="7">
         <v>42620</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="7">
         <v>42621</v>
       </c>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
     </row>
     <row r="17" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
     </row>
     <row r="22" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
     </row>
     <row r="23" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="14"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" t="s">

</xml_diff>